<commit_message>
more crap, almost done :)
</commit_message>
<xml_diff>
--- a/Output/Tables/table 2 - congestion by duid top 10.xlsx
+++ b/Output/Tables/table 2 - congestion by duid top 10.xlsx
@@ -9,48 +9,33 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
-    <sheet name="congestion by duid top 10 - ass" sheetId="1" r:id="rId1"/>
+    <sheet name="congestion by duid top 10" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
-  <si>
-    <t>station</t>
-  </si>
-  <si>
-    <t>fuel_type</t>
-  </si>
-  <si>
-    <t>perc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+  <si>
+    <t>Lake Bonney Stage 2</t>
+  </si>
+  <si>
+    <t>Wind</t>
   </si>
   <si>
     <t>Lake Bonney Stage 3</t>
   </si>
   <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Lake Bonney Stage 2</t>
-  </si>
-  <si>
     <t>Snowtown North Wind Farm</t>
   </si>
   <si>
     <t>Snowtown South Wind Farm</t>
   </si>
   <si>
-    <t>Murray</t>
-  </si>
-  <si>
-    <t>Hydro</t>
-  </si>
-  <si>
     <t>Hallett Wind Farm</t>
   </si>
   <si>
@@ -64,13 +49,28 @@
   </si>
   <si>
     <t>Snowtown Wind Farm</t>
+  </si>
+  <si>
+    <t>Clements Gap Wind Farm</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,15 +201,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -556,9 +547,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -883,137 +875,139 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0.16462138508371399</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15.598363774733601</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>0.16454528158295301</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15.1522070015221</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0.13789954337899499</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>13.6339421613394</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0.13789954337899499</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>13.632039573820402</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>0.13357115677321199</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>13.165905631659101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>0.13203957382039599</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>13.112633181126302</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>0.131858828006088</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12.991818873668201</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.13032724505327201</v>
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12.950913242009099</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>0.13032724505327201</v>
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12.8491248097412</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0.12873858447488601</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>12.706430745814302</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>